<commit_message>
added documentation for classes added another demo track and synth instrument minor formatting improvements
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calum\Desktop\Random Code\synth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calum\Desktop\Code\synth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A90177B-C1A1-4F26-B103-3C26EFA4F58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8639870-5B80-4F48-9AC6-FDF6C36A6858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{015601A0-6327-4433-AF1C-8580EBCF8248}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{015601A0-6327-4433-AF1C-8580EBCF8248}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo" sheetId="2" r:id="rId1"/>
+    <sheet name="Megalovania" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="34">
   <si>
     <t>|</t>
   </si>
@@ -111,6 +112,33 @@
   </si>
   <si>
     <t>arp.0</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>lead2.0</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>a#2</t>
   </si>
 </sst>
 </file>
@@ -483,16 +511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BD454E-081A-411E-BBD6-D724784B8A45}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.23046875" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -516,7 +544,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -542,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -566,7 +594,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -590,7 +618,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -614,7 +642,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -638,7 +666,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -662,7 +690,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -686,7 +714,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -710,7 +738,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -734,7 +762,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -758,7 +786,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -782,7 +810,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -806,7 +834,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -830,7 +858,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -854,7 +882,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -878,7 +906,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -902,7 +930,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -926,7 +954,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -950,7 +978,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -974,7 +1002,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1026,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1050,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1074,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1098,7 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1122,7 @@
       </c>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1146,7 @@
       </c>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1170,7 @@
       </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +1194,7 @@
       </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1218,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1242,7 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1266,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1290,7 @@
       </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1314,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1312,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1364,7 @@
       </c>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1388,7 @@
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1412,7 @@
       </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1436,7 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1460,7 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1484,7 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1508,7 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1504,7 +1532,7 @@
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1556,7 @@
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1552,7 +1580,7 @@
       </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1604,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1600,7 +1628,7 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1652,7 @@
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1676,7 @@
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +1700,7 @@
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -1696,7 +1724,7 @@
       </c>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -1720,7 +1748,7 @@
       </c>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1772,7 @@
       </c>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1796,7 @@
       </c>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1820,7 @@
       </c>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -1816,7 +1844,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1868,7 @@
       </c>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +1892,7 @@
       </c>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -1888,7 +1916,7 @@
       </c>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1940,7 @@
       </c>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -1936,7 +1964,7 @@
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1988,7 @@
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -1984,7 +2012,7 @@
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2008,7 +2036,7 @@
       </c>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2060,7 @@
       </c>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -2055,7 +2083,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>16</v>
       </c>
@@ -2081,7 +2109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>0</v>
       </c>
@@ -2105,7 +2133,7 @@
       </c>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2157,7 @@
       </c>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>0</v>
       </c>
@@ -2153,7 +2181,7 @@
       </c>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>0</v>
       </c>
@@ -2177,7 +2205,7 @@
       </c>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>0</v>
       </c>
@@ -2201,7 +2229,7 @@
       </c>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>0</v>
       </c>
@@ -2225,7 +2253,7 @@
       </c>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2277,7 @@
       </c>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>0</v>
       </c>
@@ -2273,7 +2301,7 @@
       </c>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>0</v>
       </c>
@@ -2297,7 +2325,7 @@
       </c>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>0</v>
       </c>
@@ -2321,7 +2349,7 @@
       </c>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>0</v>
       </c>
@@ -2345,7 +2373,7 @@
       </c>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>0</v>
       </c>
@@ -2369,7 +2397,7 @@
       </c>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2421,7 @@
       </c>
       <c r="H79" s="3"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>0</v>
       </c>
@@ -2417,7 +2445,7 @@
       </c>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>0</v>
       </c>
@@ -2441,7 +2469,7 @@
       </c>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>0</v>
       </c>
@@ -2465,7 +2493,7 @@
       </c>
       <c r="H82" s="3"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2517,7 @@
       </c>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2541,7 @@
       </c>
       <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>0</v>
       </c>
@@ -2537,7 +2565,7 @@
       </c>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2589,7 @@
       </c>
       <c r="H86" s="3"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>0</v>
       </c>
@@ -2585,7 +2613,7 @@
       </c>
       <c r="H87" s="3"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +2637,7 @@
       </c>
       <c r="H88" s="3"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>0</v>
       </c>
@@ -2633,7 +2661,7 @@
       </c>
       <c r="H89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>0</v>
       </c>
@@ -2657,7 +2685,7 @@
       </c>
       <c r="H90" s="3"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>0</v>
       </c>
@@ -2681,7 +2709,7 @@
       </c>
       <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>0</v>
       </c>
@@ -2705,7 +2733,7 @@
       </c>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>0</v>
       </c>
@@ -2729,7 +2757,7 @@
       </c>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>0</v>
       </c>
@@ -2753,7 +2781,7 @@
       </c>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>0</v>
       </c>
@@ -2777,7 +2805,7 @@
       </c>
       <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>0</v>
       </c>
@@ -2801,7 +2829,7 @@
       </c>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>0</v>
       </c>
@@ -2825,7 +2853,7 @@
       </c>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>1</v>
       </c>
@@ -2852,7 +2880,7 @@
       </c>
       <c r="I98" s="3"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>0</v>
       </c>
@@ -2876,7 +2904,7 @@
       </c>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>0</v>
       </c>
@@ -2900,7 +2928,7 @@
       </c>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>0</v>
       </c>
@@ -2924,7 +2952,7 @@
       </c>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>0</v>
       </c>
@@ -2948,7 +2976,7 @@
       </c>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>0</v>
       </c>
@@ -2972,7 +3000,7 @@
       </c>
       <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>0</v>
       </c>
@@ -2996,7 +3024,7 @@
       </c>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>0</v>
       </c>
@@ -3020,7 +3048,7 @@
       </c>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +3072,7 @@
       </c>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +3096,7 @@
       </c>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>0</v>
       </c>
@@ -3092,7 +3120,7 @@
       </c>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>0</v>
       </c>
@@ -3116,7 +3144,7 @@
       </c>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>0</v>
       </c>
@@ -3140,7 +3168,7 @@
       </c>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>0</v>
       </c>
@@ -3164,7 +3192,7 @@
       </c>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3216,7 @@
       </c>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>0</v>
       </c>
@@ -3212,7 +3240,7 @@
       </c>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3264,7 @@
       </c>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>0</v>
       </c>
@@ -3260,7 +3288,7 @@
       </c>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>0</v>
       </c>
@@ -3284,7 +3312,7 @@
       </c>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>0</v>
       </c>
@@ -3308,7 +3336,7 @@
       </c>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>0</v>
       </c>
@@ -3332,7 +3360,7 @@
       </c>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>0</v>
       </c>
@@ -3356,7 +3384,7 @@
       </c>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>0</v>
       </c>
@@ -3380,7 +3408,7 @@
       </c>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>0</v>
       </c>
@@ -3404,7 +3432,7 @@
       </c>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>0</v>
       </c>
@@ -3428,7 +3456,7 @@
       </c>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +3480,7 @@
       </c>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>0</v>
       </c>
@@ -3476,7 +3504,7 @@
       </c>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>0</v>
       </c>
@@ -3500,7 +3528,7 @@
       </c>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>0</v>
       </c>
@@ -3524,7 +3552,7 @@
       </c>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>0</v>
       </c>
@@ -3548,7 +3576,7 @@
       </c>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +3600,7 @@
       </c>
       <c r="H128" s="3"/>
     </row>
-    <row r="129" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>0</v>
       </c>
@@ -3596,7 +3624,7 @@
       </c>
       <c r="H129" s="3"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>0</v>
       </c>
@@ -3619,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>0</v>
       </c>
@@ -3642,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>0</v>
       </c>
@@ -3665,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>0</v>
       </c>
@@ -3688,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>0</v>
       </c>
@@ -3711,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>0</v>
       </c>
@@ -3734,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>0</v>
       </c>
@@ -3757,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>0</v>
       </c>
@@ -3780,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>0</v>
       </c>
@@ -3803,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>0</v>
       </c>
@@ -3826,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>0</v>
       </c>
@@ -3849,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>0</v>
       </c>
@@ -3872,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>0</v>
       </c>
@@ -3895,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>0</v>
       </c>
@@ -3918,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>0</v>
       </c>
@@ -3938,6 +3966,1372 @@
         <v>0</v>
       </c>
       <c r="G144" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50B2003-62CE-4EC8-B2A2-B63704948E3E}">
+  <dimension ref="A1:D129"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>25</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B95" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B99" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B101" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>29</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B105" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>27</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B110" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B111" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>17</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>25</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B125" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>